<commit_message>
- NhapHang: get + bind mauin {NccVanChuyen}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_PhieuNhapHang.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_PhieuNhapHang.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Ghi chú</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Giá trị sau trả</t>
+  </si>
+  <si>
+    <t>Tên NCC vận chuyển</t>
+  </si>
+  <si>
+    <t>Đã chi bên v/c</t>
   </si>
 </sst>
 </file>
@@ -167,7 +173,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -303,39 +309,40 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="39" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -642,12 +649,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,49 +668,52 @@
     <col min="7" max="7" width="25.28515625" style="8" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="6" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" style="34" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="26" customWidth="1"/>
     <col min="11" max="12" width="19.7109375" style="22" customWidth="1"/>
     <col min="13" max="13" width="19.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="22" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="18.140625" style="22" customWidth="1"/>
-    <col min="22" max="22" width="21.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.7109375" style="22" customWidth="1"/>
-    <col min="24" max="24" width="21.7109375" style="11" customWidth="1"/>
-    <col min="25" max="25" width="17.85546875" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="25.85546875" style="8" customWidth="1"/>
+    <col min="15" max="16" width="19.140625" style="22" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="18.140625" style="22" customWidth="1"/>
+    <col min="24" max="24" width="21.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.7109375" style="22" customWidth="1"/>
+    <col min="26" max="26" width="21.7109375" style="11" customWidth="1"/>
+    <col min="27" max="27" width="17.85546875" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="5"/>
-    </row>
-    <row r="4" spans="1:25" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="5"/>
+    </row>
+    <row r="4" spans="1:27" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -743,44 +753,50 @@
       <c r="M4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="P4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="R4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="S4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="T4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="U4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="V4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="20" t="s">
+      <c r="W4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="20" t="s">
+      <c r="X4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="W4" s="20" t="s">
+      <c r="Y4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="X4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="9" t="s">
+      <c r="Z4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -789,12 +805,12 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="33"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="25"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
+      <c r="N5" s="10"/>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
       <c r="Q5" s="21"/>
@@ -804,10 +820,12 @@
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
       <c r="W5" s="21"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="18"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="18"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -816,12 +834,12 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="17"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="33"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="25"/>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
+      <c r="N6" s="10"/>
       <c r="O6" s="21"/>
       <c r="P6" s="21"/>
       <c r="Q6" s="21"/>
@@ -831,10 +849,12 @@
       <c r="U6" s="21"/>
       <c r="V6" s="21"/>
       <c r="W6" s="21"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="18"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X6" s="21"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="18"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -843,12 +863,12 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="17"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="33"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="25"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
+      <c r="N7" s="10"/>
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
       <c r="Q7" s="21"/>
@@ -858,10 +878,12 @@
       <c r="U7" s="21"/>
       <c r="V7" s="21"/>
       <c r="W7" s="21"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="18"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="18"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -870,12 +892,12 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="17"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="33"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
+      <c r="N8" s="10"/>
       <c r="O8" s="21"/>
       <c r="P8" s="21"/>
       <c r="Q8" s="21"/>
@@ -885,10 +907,12 @@
       <c r="U8" s="21"/>
       <c r="V8" s="21"/>
       <c r="W8" s="21"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="18"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="18"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -897,12 +921,12 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="17"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="33"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
+      <c r="N9" s="10"/>
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="21"/>
@@ -912,10 +936,12 @@
       <c r="U9" s="21"/>
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="18"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="18"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -924,12 +950,12 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="33"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
+      <c r="N10" s="10"/>
       <c r="O10" s="21"/>
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
@@ -939,10 +965,12 @@
       <c r="U10" s="21"/>
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
-      <c r="X10" s="12"/>
-      <c r="Y10" s="18"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="18"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -951,12 +979,12 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="33"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="25"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
+      <c r="N11" s="10"/>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="21"/>
@@ -966,10 +994,12 @@
       <c r="U11" s="21"/>
       <c r="V11" s="21"/>
       <c r="W11" s="21"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="18"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="18"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -978,12 +1008,12 @@
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="33"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="25"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
+      <c r="N12" s="10"/>
       <c r="O12" s="21"/>
       <c r="P12" s="21"/>
       <c r="Q12" s="21"/>
@@ -993,10 +1023,12 @@
       <c r="U12" s="21"/>
       <c r="V12" s="21"/>
       <c r="W12" s="21"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="18"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="18"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1005,12 +1037,12 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="33"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="25"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
+      <c r="N13" s="10"/>
       <c r="O13" s="21"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
@@ -1020,10 +1052,12 @@
       <c r="U13" s="21"/>
       <c r="V13" s="21"/>
       <c r="W13" s="21"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="18"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="18"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1032,12 +1066,12 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="17"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="33"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
+      <c r="N14" s="10"/>
       <c r="O14" s="21"/>
       <c r="P14" s="21"/>
       <c r="Q14" s="21"/>
@@ -1047,10 +1081,12 @@
       <c r="U14" s="21"/>
       <c r="V14" s="21"/>
       <c r="W14" s="21"/>
-      <c r="X14" s="12"/>
-      <c r="Y14" s="18"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X14" s="21"/>
+      <c r="Y14" s="21"/>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="18"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1059,12 +1095,12 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="33"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
+      <c r="N15" s="10"/>
       <c r="O15" s="21"/>
       <c r="P15" s="21"/>
       <c r="Q15" s="21"/>
@@ -1074,10 +1110,12 @@
       <c r="U15" s="21"/>
       <c r="V15" s="21"/>
       <c r="W15" s="21"/>
-      <c r="X15" s="12"/>
-      <c r="Y15" s="18"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X15" s="21"/>
+      <c r="Y15" s="21"/>
+      <c r="Z15" s="12"/>
+      <c r="AA15" s="18"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1086,12 +1124,12 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="17"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
+      <c r="N16" s="10"/>
       <c r="O16" s="21"/>
       <c r="P16" s="21"/>
       <c r="Q16" s="21"/>
@@ -1101,10 +1139,12 @@
       <c r="U16" s="21"/>
       <c r="V16" s="21"/>
       <c r="W16" s="21"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="18"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="18"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -1113,12 +1153,12 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="33"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="25"/>
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
+      <c r="N17" s="10"/>
       <c r="O17" s="21"/>
       <c r="P17" s="21"/>
       <c r="Q17" s="21"/>
@@ -1128,10 +1168,12 @@
       <c r="U17" s="21"/>
       <c r="V17" s="21"/>
       <c r="W17" s="21"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="18"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X17" s="21"/>
+      <c r="Y17" s="21"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="18"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1140,12 +1182,12 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="33"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
+      <c r="N18" s="10"/>
       <c r="O18" s="21"/>
       <c r="P18" s="21"/>
       <c r="Q18" s="21"/>
@@ -1155,10 +1197,12 @@
       <c r="U18" s="21"/>
       <c r="V18" s="21"/>
       <c r="W18" s="21"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="18"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="18"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1167,12 +1211,12 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="33"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
+      <c r="N19" s="10"/>
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="21"/>
@@ -1182,10 +1226,12 @@
       <c r="U19" s="21"/>
       <c r="V19" s="21"/>
       <c r="W19" s="21"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="18"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X19" s="21"/>
+      <c r="Y19" s="21"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="18"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -1194,12 +1240,12 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="33"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
+      <c r="N20" s="10"/>
       <c r="O20" s="21"/>
       <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
@@ -1209,10 +1255,12 @@
       <c r="U20" s="21"/>
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
-      <c r="X20" s="12"/>
-      <c r="Y20" s="18"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X20" s="21"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="18"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1221,12 +1269,12 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="33"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
+      <c r="N21" s="10"/>
       <c r="O21" s="21"/>
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
@@ -1236,10 +1284,12 @@
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="18"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X21" s="21"/>
+      <c r="Y21" s="21"/>
+      <c r="Z21" s="12"/>
+      <c r="AA21" s="18"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -1248,12 +1298,12 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="17"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="33"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
+      <c r="N22" s="10"/>
       <c r="O22" s="21"/>
       <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
@@ -1263,10 +1313,12 @@
       <c r="U22" s="21"/>
       <c r="V22" s="21"/>
       <c r="W22" s="21"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="18"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X22" s="21"/>
+      <c r="Y22" s="21"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="18"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -1275,12 +1327,12 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="17"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="33"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="25"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
+      <c r="N23" s="10"/>
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
@@ -1290,10 +1342,12 @@
       <c r="U23" s="21"/>
       <c r="V23" s="21"/>
       <c r="W23" s="21"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="18"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X23" s="21"/>
+      <c r="Y23" s="21"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="18"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -1302,12 +1356,12 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="17"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="33"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
+      <c r="N24" s="10"/>
       <c r="O24" s="21"/>
       <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
@@ -1317,10 +1371,12 @@
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
-      <c r="X24" s="12"/>
-      <c r="Y24" s="18"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X24" s="21"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24" s="12"/>
+      <c r="AA24" s="18"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -1329,12 +1385,12 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="17"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="33"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25"/>
       <c r="K25" s="21"/>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
+      <c r="N25" s="10"/>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
       <c r="Q25" s="21"/>
@@ -1344,10 +1400,12 @@
       <c r="U25" s="21"/>
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
-      <c r="X25" s="12"/>
-      <c r="Y25" s="18"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="12"/>
+      <c r="AA25" s="18"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1356,12 +1414,12 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="17"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="33"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25"/>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
+      <c r="N26" s="10"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21"/>
       <c r="Q26" s="21"/>
@@ -1371,10 +1429,12 @@
       <c r="U26" s="21"/>
       <c r="V26" s="21"/>
       <c r="W26" s="21"/>
-      <c r="X26" s="12"/>
-      <c r="Y26" s="18"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="18"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1383,12 +1443,12 @@
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="17"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="33"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="25"/>
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
+      <c r="N27" s="10"/>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
       <c r="Q27" s="21"/>
@@ -1398,10 +1458,12 @@
       <c r="U27" s="21"/>
       <c r="V27" s="21"/>
       <c r="W27" s="21"/>
-      <c r="X27" s="12"/>
-      <c r="Y27" s="18"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X27" s="21"/>
+      <c r="Y27" s="21"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="18"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1410,12 +1472,12 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="17"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="33"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
+      <c r="N28" s="10"/>
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
       <c r="Q28" s="21"/>
@@ -1425,19 +1487,21 @@
       <c r="U28" s="21"/>
       <c r="V28" s="21"/>
       <c r="W28" s="21"/>
-      <c r="X28" s="12"/>
-      <c r="Y28" s="18"/>
-    </row>
-    <row r="29" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="29">
+      <c r="X28" s="21"/>
+      <c r="Y28" s="21"/>
+      <c r="Z28" s="12"/>
+      <c r="AA28" s="18"/>
+    </row>
+    <row r="29" spans="1:27" s="34" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="30">
         <f xml:space="preserve"> SUM(I$5:I28)</f>
         <v>0</v>
       </c>
@@ -1457,10 +1521,7 @@
         <f xml:space="preserve"> SUM(M$5:M28)</f>
         <v>0</v>
       </c>
-      <c r="N29" s="31">
-        <f xml:space="preserve"> SUM(N$5:N28)</f>
-        <v>0</v>
-      </c>
+      <c r="N29" s="35"/>
       <c r="O29" s="31">
         <f xml:space="preserve"> SUM(O$5:O28)</f>
         <v>0</v>
@@ -1497,12 +1558,20 @@
         <f xml:space="preserve"> SUM(W$5:W28)</f>
         <v>0</v>
       </c>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="27"/>
+      <c r="X29" s="31">
+        <f xml:space="preserve"> SUM(X$5:X28)</f>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="31">
+        <f xml:space="preserve"> SUM(Y$5:Y28)</f>
+        <v>0</v>
+      </c>
+      <c r="Z29" s="32"/>
+      <c r="AA29" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A1:X1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>